<commit_message>
As of March 4, 12:30AM
</commit_message>
<xml_diff>
--- a/Participants.xlsx
+++ b/Participants.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ijJPN2\Documents\NetBeansProjects\DARBMS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
@@ -51,7 +56,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -96,11 +101,42 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -149,7 +185,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -182,9 +218,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -217,6 +270,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -396,10 +466,15 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
3/24/2018 8:11AM - Updates
</commit_message>
<xml_diff>
--- a/Participants.xlsx
+++ b/Participants.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ijJPN2\Documents\NetBeansProjects\DARBMS\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
@@ -16,12 +11,15 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Last Name</t>
   </si>
@@ -32,31 +30,46 @@
     <t>Middle Name</t>
   </si>
   <si>
-    <t>Hood</t>
-  </si>
-  <si>
-    <t>Clarkson</t>
-  </si>
-  <si>
-    <t>Nance</t>
-  </si>
-  <si>
-    <t>Rodney</t>
-  </si>
-  <si>
-    <t>James</t>
-  </si>
-  <si>
-    <t>Jordan</t>
-  </si>
-  <si>
-    <t>Larry</t>
+    <t>Gamboa</t>
+  </si>
+  <si>
+    <t>Rey Christian</t>
+  </si>
+  <si>
+    <t>Lopez</t>
+  </si>
+  <si>
+    <t>Francisco</t>
+  </si>
+  <si>
+    <t>Christopher Jorge</t>
+  </si>
+  <si>
+    <t>Pineda</t>
+  </si>
+  <si>
+    <t>Naguit</t>
+  </si>
+  <si>
+    <t>Lanz</t>
+  </si>
+  <si>
+    <t>Pundavela</t>
+  </si>
+  <si>
+    <t>Calantuan</t>
+  </si>
+  <si>
+    <t>Earle</t>
+  </si>
+  <si>
+    <t>LeBron</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -185,7 +198,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -218,26 +231,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -270,23 +266,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -463,16 +442,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -492,32 +471,43 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>